<commit_message>
Configuration finally done with mostly
Finished up the methods for parsing out the configuration data from the
input Excel file. Also removed the Course class because it was useless,
and renamed a few things for better clarity.
</commit_message>
<xml_diff>
--- a/demo/IO Spec Input.xlsx
+++ b/demo/IO Spec Input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Course Equivelents" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Course Equivalents" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Course Areas" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Grade Schema" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Rank Schema" sheetId="4" state="visible" r:id="rId5"/>
@@ -740,7 +740,7 @@
   </sheetPr>
   <dimension ref="A1:AH4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1672,7 +1672,7 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>